<commit_message>
Added request table near the schedule for easy access
</commit_message>
<xml_diff>
--- a/Template/תבנית סידור.xlsx
+++ b/Template/תבנית סידור.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3972" yWindow="996" windowWidth="17280" windowHeight="8880" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -63,7 +63,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -102,14 +102,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0098FB98"/>
-        <bgColor rgb="0098FB98"/>
+        <fgColor rgb="FF98FB98"/>
+        <bgColor rgb="FF98FB98"/>
       </patternFill>
     </fill>
   </fills>
@@ -194,7 +188,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
@@ -237,9 +231,9 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
@@ -251,7 +245,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,22 +589,24 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="C10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J10" sqref="J2:J10"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="15.6640625" customWidth="1" min="2" max="2"/>
-    <col width="14.6640625" customWidth="1" min="3" max="3"/>
-    <col width="14.33203125" customWidth="1" min="4" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="14.33203125" customWidth="1" min="7" max="7"/>
-    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="11.6640625" customWidth="1" min="1" max="1"/>
+    <col width="6.109375" customWidth="1" min="2" max="2"/>
+    <col width="7.5546875" customWidth="1" min="3" max="3"/>
+    <col width="6.44140625" customWidth="1" min="4" max="4"/>
+    <col width="8.44140625" customWidth="1" min="5" max="5"/>
+    <col width="7.109375" customWidth="1" min="6" max="6"/>
+    <col width="6.33203125" customWidth="1" min="7" max="7"/>
+    <col width="6.77734375" customWidth="1" min="8" max="8"/>
     <col width="2.5546875" customWidth="1" min="9" max="9"/>
+    <col width="3.33203125" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -627,9 +622,49 @@
       <c r="F1" s="22" t="n"/>
       <c r="G1" s="22" t="n"/>
       <c r="H1" s="23" t="n"/>
-      <c r="J1" s="19" t="inlineStr">
+      <c r="J1" s="18" t="inlineStr">
         <is>
           <t>שמות:</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>א</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>ב</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>ג</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>ד</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>ה</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>ו</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>ש</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>כמות משמרות:</t>
         </is>
       </c>
     </row>
@@ -674,10 +709,53 @@
           <t>שבת 16.3</t>
         </is>
       </c>
-      <c r="J2" s="20" t="inlineStr">
+      <c r="J2" s="19" t="inlineStr">
         <is>
           <t>זיו</t>
         </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>זיו</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>a.b</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>b.c</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>a.b</t>
+        </is>
+      </c>
+      <c r="T2" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -698,6 +776,49 @@
           <t>אור</t>
         </is>
       </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>אור</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>b.c</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="T3" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="14" t="inlineStr">
@@ -717,6 +838,49 @@
           <t>רוני</t>
         </is>
       </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>רוני</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>a.b</t>
+        </is>
+      </c>
+      <c r="T4" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="15" t="inlineStr">
@@ -736,6 +900,39 @@
           <t xml:space="preserve">אמור </t>
         </is>
       </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">אמור </t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>a.c</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>a.b</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="T5" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="15" t="inlineStr">
@@ -755,6 +952,49 @@
           <t>אוראל</t>
         </is>
       </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>אוראל</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>b.c</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>b.c</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="T6" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="21" t="inlineStr">
@@ -774,6 +1014,39 @@
           <t>יניב</t>
         </is>
       </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>יניב</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>a.b</t>
+        </is>
+      </c>
+      <c r="T7" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="16" t="inlineStr">
@@ -793,6 +1066,39 @@
           <t>עמית</t>
         </is>
       </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>עמית</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>a.c</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>a.c</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="T8" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="15" t="inlineStr">
@@ -807,7 +1113,7 @@
       <c r="F9" s="6" t="n"/>
       <c r="G9" s="7" t="n"/>
       <c r="H9" s="7" t="n"/>
-      <c r="J9" s="26" t="inlineStr">
+      <c r="J9" s="20" t="inlineStr">
         <is>
           <t>תגבור</t>
         </is>

</xml_diff>

<commit_message>
Clear title and color for the schedule
</commit_message>
<xml_diff>
--- a/Template/תבנית סידור.xlsx
+++ b/Template/תבנית סידור.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orbac\Desktop\Shift-Schedule\Shift-Schedule\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DEA7DBE-B8D5-4459-B2D6-E4075A49B2DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9A6B27-D82A-478B-B55E-B8D79B981B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4380" yWindow="4680" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>סידור עבודה צוות עדי</t>
   </si>
@@ -68,6 +68,36 @@
   </si>
   <si>
     <t>הערות</t>
+  </si>
+  <si>
+    <t>הערות:</t>
+  </si>
+  <si>
+    <t>א</t>
+  </si>
+  <si>
+    <t>ב</t>
+  </si>
+  <si>
+    <t>ג</t>
+  </si>
+  <si>
+    <t>ד</t>
+  </si>
+  <si>
+    <t>ה</t>
+  </si>
+  <si>
+    <t>ו</t>
+  </si>
+  <si>
+    <t>ש</t>
+  </si>
+  <si>
+    <t>כמות</t>
+  </si>
+  <si>
+    <t>מקס משמרות</t>
   </si>
 </sst>
 </file>
@@ -121,7 +151,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,6 +185,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -211,7 +247,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -264,6 +300,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -547,27 +587,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" customWidth="1"/>
-    <col min="3" max="3" width="6.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
     <col min="6" max="6" width="7" customWidth="1"/>
-    <col min="7" max="7" width="5.88671875" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" customWidth="1"/>
-    <col min="9" max="9" width="2.5546875" customWidth="1"/>
-    <col min="11" max="11" width="3.33203125" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" customWidth="1"/>
+    <col min="9" max="9" width="2.5703125" customWidth="1"/>
+    <col min="11" max="11" width="1.42578125" customWidth="1"/>
+    <col min="12" max="12" width="4.28515625" customWidth="1"/>
+    <col min="13" max="13" width="5.7109375" customWidth="1"/>
+    <col min="14" max="14" width="5.28515625" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" customWidth="1"/>
+    <col min="16" max="16" width="4.85546875" customWidth="1"/>
+    <col min="17" max="17" width="4.7109375" customWidth="1"/>
+    <col min="18" max="19" width="4.5703125" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -581,8 +629,38 @@
       <c r="J1" s="18" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L1" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" s="25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -608,7 +686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
@@ -620,7 +698,7 @@
       <c r="G3" s="20"/>
       <c r="H3" s="21"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>11</v>
       </c>
@@ -632,7 +710,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>12</v>
       </c>
@@ -644,7 +722,7 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>13</v>
       </c>
@@ -656,7 +734,7 @@
       <c r="G6" s="7"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>14</v>
       </c>
@@ -668,7 +746,7 @@
       <c r="G7" s="20"/>
       <c r="H7" s="21"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>11</v>
       </c>
@@ -680,7 +758,7 @@
       <c r="G8" s="5"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>12</v>
       </c>
@@ -692,7 +770,7 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>13</v>
       </c>
@@ -704,7 +782,7 @@
       <c r="G10" s="7"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>15</v>
       </c>
@@ -716,7 +794,7 @@
       <c r="G11" s="20"/>
       <c r="H11" s="21"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="2"/>
       <c r="C12" s="5"/>
@@ -726,7 +804,7 @@
       <c r="G12" s="12"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -736,7 +814,7 @@
       <c r="G13" s="8"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="1"/>
       <c r="C14" s="5"/>

</xml_diff>

<commit_message>
removed unnecessary files and code
</commit_message>
<xml_diff>
--- a/Template/תבנית סידור.xlsx
+++ b/Template/תבנית סידור.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orbac\Desktop\Shift-Schedule\Shift-Schedule\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9A6B27-D82A-478B-B55E-B8D79B981B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EABEC4-1DF7-41DF-B219-525F995D8EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="4680" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,15 +55,6 @@
     <t xml:space="preserve">עמדה כניסה </t>
   </si>
   <si>
-    <t>6:00-14:00</t>
-  </si>
-  <si>
-    <t>14:00-22:00</t>
-  </si>
-  <si>
-    <t>22:00-6:00</t>
-  </si>
-  <si>
     <t>עמדה אחורית</t>
   </si>
   <si>
@@ -98,6 +89,15 @@
   </si>
   <si>
     <t>מקס משמרות</t>
+  </si>
+  <si>
+    <t>7:00-15:00</t>
+  </si>
+  <si>
+    <t>15:00-23:00</t>
+  </si>
+  <si>
+    <t>23:00-7:00</t>
   </si>
 </sst>
 </file>
@@ -247,7 +247,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -284,13 +284,11 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -300,10 +298,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -590,32 +584,32 @@
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
     <col min="6" max="6" width="7" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" customWidth="1"/>
-    <col min="9" max="9" width="2.5703125" customWidth="1"/>
-    <col min="11" max="11" width="1.42578125" customWidth="1"/>
-    <col min="12" max="12" width="4.28515625" customWidth="1"/>
-    <col min="13" max="13" width="5.7109375" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" customWidth="1"/>
-    <col min="15" max="15" width="5.85546875" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" customWidth="1"/>
-    <col min="17" max="17" width="4.7109375" customWidth="1"/>
-    <col min="18" max="19" width="4.5703125" customWidth="1"/>
-    <col min="20" max="20" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="5.88671875" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" customWidth="1"/>
+    <col min="9" max="9" width="2.5546875" customWidth="1"/>
+    <col min="11" max="11" width="1.44140625" customWidth="1"/>
+    <col min="12" max="12" width="4.33203125" customWidth="1"/>
+    <col min="13" max="13" width="5.6640625" customWidth="1"/>
+    <col min="14" max="14" width="5.33203125" customWidth="1"/>
+    <col min="15" max="15" width="5.88671875" customWidth="1"/>
+    <col min="16" max="16" width="4.88671875" customWidth="1"/>
+    <col min="17" max="17" width="4.6640625" customWidth="1"/>
+    <col min="18" max="19" width="4.5546875" customWidth="1"/>
+    <col min="20" max="20" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -626,41 +620,41 @@
       <c r="F1" s="20"/>
       <c r="G1" s="20"/>
       <c r="H1" s="21"/>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="L1" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="P1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="Q1" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="25" t="s">
+      <c r="R1" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="25" t="s">
+      <c r="S1" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="25" t="s">
+      <c r="T1" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="U1" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="S1" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="T1" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" s="25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -686,7 +680,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
@@ -698,9 +692,9 @@
       <c r="G3" s="20"/>
       <c r="H3" s="21"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="6"/>
@@ -710,9 +704,9 @@
       <c r="G4" s="5"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -722,9 +716,9 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -734,9 +728,9 @@
       <c r="G6" s="7"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -746,9 +740,9 @@
       <c r="G7" s="20"/>
       <c r="H7" s="21"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>11</v>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>23</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -758,9 +752,9 @@
       <c r="G8" s="5"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -770,9 +764,9 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>13</v>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
+        <v>25</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
@@ -782,9 +776,9 @@
       <c r="G10" s="7"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
@@ -794,7 +788,7 @@
       <c r="G11" s="20"/>
       <c r="H11" s="21"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="2"/>
       <c r="C12" s="5"/>
@@ -804,7 +798,7 @@
       <c r="G12" s="12"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -814,7 +808,7 @@
       <c r="G13" s="8"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
       <c r="B14" s="1"/>
       <c r="C14" s="5"/>

</xml_diff>